<commit_message>
Started acceptance criteria 2, but needs your feedback
</commit_message>
<xml_diff>
--- a/src/test/resources/datasets/NAMIS-TestCase_registerSFCwhenSFOalreadyExists.xlsx
+++ b/src/test/resources/datasets/NAMIS-TestCase_registerSFCwhenSFOalreadyExists.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FO_Cycle</t>
   </si>
@@ -35,16 +34,13 @@
     <t>Num_Received_Apps</t>
   </si>
   <si>
+    <t>SAMPLE EN</t>
+  </si>
+  <si>
+    <t>SAMPLE FR</t>
+  </si>
+  <si>
     <t>SAMPLE-2009</t>
-  </si>
-  <si>
-    <t>SAMPLE</t>
-  </si>
-  <si>
-    <t>SAMPLE EN</t>
-  </si>
-  <si>
-    <t>SAMPLE FR</t>
   </si>
 </sst>
 </file>
@@ -376,7 +372,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -411,19 +407,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>2009</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="2">
         <v>3</v>
@@ -485,39 +478,39 @@
       <c r="B16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="2:6">
       <c r="B17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="2:6">
       <c r="B18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="2:6">
       <c r="B19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="2:6">
       <c r="B20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="2:6">
       <c r="B21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="2:6">
       <c r="B22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="2:6">
       <c r="B23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="2:6">
       <c r="B24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="2:6">
       <c r="B25" s="2"/>
       <c r="F25" s="2"/>
     </row>

</xml_diff>

<commit_message>
adjusted test_applyChangesFromFileByIds_regsiterSFCwhenSFOalreadyExists, but still needs work.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasets/NAMIS-TestCase_registerSFCwhenSFOalreadyExists.xlsx
+++ b/src/test/resources/datasets/NAMIS-TestCase_registerSFCwhenSFOalreadyExists.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="19275" windowHeight="7080"/>
+    <workbookView xWindow="-3285" yWindow="105" windowWidth="14940" windowHeight="3765"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>FO_Cycle</t>
   </si>
@@ -41,6 +42,9 @@
   </si>
   <si>
     <t>SAMPLE-2009</t>
+  </si>
+  <si>
+    <t>SAMPLE</t>
   </si>
 </sst>
 </file>
@@ -372,7 +376,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -412,6 +416,9 @@
       <c r="B2" s="2">
         <v>2009</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>

</xml_diff>